<commit_message>
Avgsalary for all mun (2008-2022)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/features4superset.xlsx
+++ b/migforecasting/datasets/superdataset/features4superset.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>категория</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Миг. сальдо - saldo (чел.) (id8112021 - id8112022)</t>
+  </si>
+  <si>
+    <t>Ср. числ. работн. орг. -  avgemployers (чел.) (id8123005)</t>
+  </si>
+  <si>
+    <t>Сред. зп. - avgsalary (руб.) (id8123007)</t>
   </si>
 </sst>
 </file>
@@ -372,14 +378,14 @@
   <dimension ref="B3:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="50.7109375" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
@@ -400,10 +406,16 @@
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Shops area for all mun (2006-2023)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/features4superset.xlsx
+++ b/migforecasting/datasets/superdataset/features4superset.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>категория</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>Сред. зп. - avgsalary (руб.) (id8123007)</t>
+  </si>
+  <si>
+    <t>Торговля</t>
+  </si>
+  <si>
+    <t>Площ. торг. зал. маг. - shoparea (кв.м.) (id8002002)</t>
   </si>
 </sst>
 </file>
@@ -67,15 +73,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -83,18 +101,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -375,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D5"/>
+  <dimension ref="B3:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,9 +437,10 @@
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="50.7109375" customWidth="1"/>
     <col min="4" max="4" width="52.28515625" customWidth="1"/>
+    <col min="5" max="5" width="51" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -398,25 +450,39 @@
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Retailturnover for all mun
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/features4superset.xlsx
+++ b/migforecasting/datasets/superdataset/features4superset.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>категория</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Кол-во мест в рест,каф,бар - foodseats (место) (id8002004)</t>
+  </si>
+  <si>
+    <t>Обор. роз. (кроме авто.) - retailturnover (тыс. руб.) (id8201003)</t>
+  </si>
+  <si>
+    <t>Обор. Общепит - foodservturnover (тыс. руб.) (id8201006)</t>
   </si>
 </sst>
 </file>
@@ -136,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -148,7 +154,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -432,7 +437,7 @@
   <dimension ref="B3:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +445,7 @@
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="50.7109375" customWidth="1"/>
     <col min="4" max="4" width="52.28515625" customWidth="1"/>
-    <col min="5" max="5" width="56.5703125" customWidth="1"/>
+    <col min="5" max="5" width="66.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
@@ -484,10 +489,14 @@
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E6" s="5"/>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E7" s="5"/>
+      <c r="E7" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Consnewareas for all mun
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/features4superset.xlsx
+++ b/migforecasting/datasets/superdataset/features4superset.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>категория</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Обор. Общепит - foodservturnover (тыс. руб.) (id8201006)</t>
+  </si>
+  <si>
+    <t>Строительство</t>
+  </si>
+  <si>
+    <t>Введ. жил. дом. - consnewareas (кв. м.) (id8010001)</t>
   </si>
 </sst>
 </file>
@@ -434,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E7"/>
+  <dimension ref="B3:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,6 +504,26 @@
         <v>12</v>
       </c>
     </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Consnewapt for all mun
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/features4superset.xlsx
+++ b/migforecasting/datasets/superdataset/features4superset.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>категория</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Введ. жил. дом. - consnewareas (кв. м.) (id8010001)</t>
+  </si>
+  <si>
+    <t>Введ. кварт. - consnewapt (шт. на 1000 чел.) (id8215002)</t>
   </si>
 </sst>
 </file>
@@ -156,10 +159,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -443,7 +446,7 @@
   <dimension ref="B3:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,7 +478,7 @@
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -483,11 +486,11 @@
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -521,8 +524,10 @@
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Livarea for all mun (2007-2022)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/features4superset.xlsx
+++ b/migforecasting/datasets/superdataset/features4superset.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>категория</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>Введ. кварт. - consnewapt (шт. на 1000 чел.) (id8215002)</t>
+  </si>
+  <si>
+    <t>Уровень жизни</t>
+  </si>
+  <si>
+    <t>Жил. площ.на одного чел. - livarea (кв. м) (id8211001)</t>
   </si>
 </sst>
 </file>
@@ -446,7 +452,7 @@
   <dimension ref="B3:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,6 +520,9 @@
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="D10" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
@@ -521,6 +530,9 @@
       </c>
       <c r="C11" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
@@ -528,6 +540,7 @@
       <c r="C12" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="D12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Number of sports venue for all mun (06-22)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/features4superset.xlsx
+++ b/migforecasting/datasets/superdataset/features4superset.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>категория</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Жил. площ.на одного чел. - livarea (кв. м) (id8211001)</t>
+  </si>
+  <si>
+    <t>Число спорт. сооруж. - sportsvenue (шт.) (id8003001)</t>
   </si>
 </sst>
 </file>
@@ -452,7 +455,7 @@
   <dimension ref="B3:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +534,7 @@
       <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -540,7 +543,9 @@
       <c r="C12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Number of sevices for all mun (06-22)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/features4superset.xlsx
+++ b/migforecasting/datasets/superdataset/features4superset.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>категория</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Число спорт. сооруж. - sportsvenue (шт.) (id8003001)</t>
+  </si>
+  <si>
+    <t>Объекты быт. обслу. - servicesnum (шт.) (id8001001 &amp; 8401011)</t>
   </si>
 </sst>
 </file>
@@ -452,17 +455,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E12"/>
+  <dimension ref="B3:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="50.7109375" customWidth="1"/>
-    <col min="4" max="4" width="52.28515625" customWidth="1"/>
+    <col min="4" max="4" width="58.140625" customWidth="1"/>
     <col min="5" max="5" width="66.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -547,6 +550,11 @@
         <v>18</v>
       </c>
     </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Length of roads (for all mun)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/features4superset.xlsx
+++ b/migforecasting/datasets/superdataset/features4superset.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>категория</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>Объекты быт. обслу. - servicesnum (шт.) (id8001001 &amp; 8401011)</t>
+  </si>
+  <si>
+    <t>Длина дорог - roadslen (км) (id8006005)</t>
+  </si>
+  <si>
+    <t>Сельское хозяйство</t>
   </si>
 </sst>
 </file>
@@ -455,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E13"/>
+  <dimension ref="B3:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,6 +535,9 @@
       <c r="D10" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="E10" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
@@ -540,6 +549,7 @@
       <c r="D11" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
@@ -549,10 +559,17 @@
       <c r="D12" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D13" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Livestock for all mun
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/features4superset.xlsx
+++ b/migforecasting/datasets/superdataset/features4superset.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>категория</t>
   </si>
@@ -33,58 +33,61 @@
     <t>признаки</t>
   </si>
   <si>
-    <t>Численность - popsize (чел.) (id 8112027)</t>
-  </si>
-  <si>
-    <t>Миг. сальдо - saldo (чел.) (id8112021 - id8112022)</t>
-  </si>
-  <si>
-    <t>Ср. числ. работн. орг. -  avgemployers (чел.) (id8123005)</t>
-  </si>
-  <si>
-    <t>Сред. зп. - avgsalary (руб.) (id8123007)</t>
-  </si>
-  <si>
     <t>Торговля</t>
   </si>
   <si>
-    <t>Площ. торг. зал. маг. - shoparea (кв.м.) (id8002002)</t>
-  </si>
-  <si>
-    <t>Кол-во мест в рест,каф,бар - foodseats (место) (id8002004)</t>
-  </si>
-  <si>
-    <t>Обор. роз. (кроме авто.) - retailturnover (тыс. руб.) (id8201003)</t>
-  </si>
-  <si>
-    <t>Обор. Общепит - foodservturnover (тыс. руб.) (id8201006)</t>
-  </si>
-  <si>
     <t>Строительство</t>
   </si>
   <si>
-    <t>Введ. жил. дом. - consnewareas (кв. м.) (id8010001)</t>
-  </si>
-  <si>
-    <t>Введ. кварт. - consnewapt (шт. на 1000 чел.) (id8215002)</t>
-  </si>
-  <si>
-    <t>Уровень жизни</t>
-  </si>
-  <si>
-    <t>Жил. площ.на одного чел. - livarea (кв. м) (id8211001)</t>
-  </si>
-  <si>
-    <t>Число спорт. сооруж. - sportsvenue (шт.) (id8003001)</t>
-  </si>
-  <si>
-    <t>Объекты быт. обслу. - servicesnum (шт.) (id8001001 &amp; 8401011)</t>
-  </si>
-  <si>
-    <t>Длина дорог - roadslen (км) (id8006005)</t>
-  </si>
-  <si>
     <t>Сельское хозяйство</t>
+  </si>
+  <si>
+    <t>Поголовье скота - livestock (сум. всех видов, шт.) (8007020)</t>
+  </si>
+  <si>
+    <t>Ср. числ. работн. орг. -  avgemployers (чел.) (8123005)</t>
+  </si>
+  <si>
+    <t>Сред. зп. - avgsalary (руб.) (8123007)</t>
+  </si>
+  <si>
+    <t>Численность - popsize (чел.) (8112027)</t>
+  </si>
+  <si>
+    <t>Миг. сальдо - saldo (чел.) (8112021 - 8112022)</t>
+  </si>
+  <si>
+    <t>Площ. торг. зал. маг. - shoparea (кв.м.) (8002002)</t>
+  </si>
+  <si>
+    <t>Кол-во мест в рест,каф,бар - foodseats (место) (8002004)</t>
+  </si>
+  <si>
+    <t>Обор. роз. (кроме авто.) - retailturnover (тыс. руб.) (8201003)</t>
+  </si>
+  <si>
+    <t>Обор. Общепит - foodservturnover (тыс. руб.) (8201006)</t>
+  </si>
+  <si>
+    <t>Введ. жил. дом. - consnewareas (кв. м.) (8010001)</t>
+  </si>
+  <si>
+    <t>Введ. кварт. - consnewapt (шт. на 1000 чел.) (8215002)</t>
+  </si>
+  <si>
+    <t>Жил. площ.на одного чел. - livarea (кв. м) (8211001)</t>
+  </si>
+  <si>
+    <t>Число спорт. сооруж. - sportsvenue (шт.) (8003001)</t>
+  </si>
+  <si>
+    <t>Объекты быт. обслу. - servicesnum (шт.) (8001001 &amp; 8401011)</t>
+  </si>
+  <si>
+    <t>Длина дорог - roadslen (км) (8006005)</t>
+  </si>
+  <si>
+    <t>Уровень жизни (разное + новое)</t>
   </si>
 </sst>
 </file>
@@ -464,7 +467,7 @@
   <dimension ref="B3:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,7 +475,7 @@
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="50.7109375" customWidth="1"/>
     <col min="4" max="4" width="58.140625" customWidth="1"/>
-    <col min="5" max="5" width="66.28515625" customWidth="1"/>
+    <col min="5" max="5" width="62.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
@@ -486,7 +489,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -494,35 +497,35 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
       <c r="C5" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E6" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E7" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
@@ -530,13 +533,13 @@
         <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -544,32 +547,34 @@
         <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D13" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D14" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Harvest for all mun
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/features4superset.xlsx
+++ b/migforecasting/datasets/superdataset/features4superset.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>категория</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Уровень жизни (разное + новое)</t>
+  </si>
+  <si>
+    <t>Урожайность овощей - harvest (цент.) (8007025)</t>
   </si>
 </sst>
 </file>
@@ -467,7 +470,7 @@
   <dimension ref="B3:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +567,9 @@
       <c r="D12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D13" s="2" t="s">

</xml_diff>

<commit_message>
Agricultural prod. for all mun
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/features4superset.xlsx
+++ b/migforecasting/datasets/superdataset/features4superset.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>категория</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Урожайность овощей - harvest (цент.) (8007025)</t>
+  </si>
+  <si>
+    <t>Продук. сельхоз. - agrprod (тыс. руб) (8007010)</t>
   </si>
 </sst>
 </file>
@@ -470,7 +473,7 @@
   <dimension ref="B3:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,7 +578,9 @@
       <c r="D13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D14" s="2" t="s">

</xml_diff>

<commit_message>
Invest for all mun
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/features4superset.xlsx
+++ b/migforecasting/datasets/superdataset/features4superset.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>категория</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>Продук. сельхоз. - agrprod (тыс. руб) (8007010)</t>
+  </si>
+  <si>
+    <t>Инвестиции</t>
+  </si>
+  <si>
+    <t>Инвест. в осн. кап. - invest (тыс. руб) (8109001)</t>
   </si>
 </sst>
 </file>
@@ -178,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -190,6 +196,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -470,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E14"/>
+  <dimension ref="B3:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,6 +596,26 @@
         <v>21</v>
       </c>
     </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>